<commit_message>
Excel export, gui and finish the project
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OBH" sheetId="1" state="visible" r:id="rId2"/>
@@ -869,11 +869,11 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L50" activeCellId="0" sqref="L50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
@@ -1010,13 +1010,14 @@
         <v>27</v>
       </c>
       <c r="L3" s="14" t="n">
-        <v>6075</v>
+        <v>300</v>
       </c>
       <c r="M3" s="14" t="n">
         <v>1640.25</v>
       </c>
       <c r="N3" s="14" t="n">
-        <v>7715.25</v>
+        <f aca="false">+L3*1.27</f>
+        <v>381</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>1</v>
@@ -1039,7 +1040,7 @@
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>21114999</v>
+        <v>21114998</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>22</v>
@@ -1072,13 +1073,14 @@
         <v>27</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>12591</v>
+        <v>400</v>
       </c>
       <c r="M4" s="14" t="n">
         <v>3399.57</v>
       </c>
       <c r="N4" s="14" t="n">
-        <v>15990.57</v>
+        <f aca="false">+L4*1.27</f>
+        <v>508</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>1</v>
@@ -3992,11 +3994,11 @@
   </sheetPr>
   <dimension ref="A1:T1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.29"/>
@@ -4133,13 +4135,14 @@
         <v>27</v>
       </c>
       <c r="L3" s="14" t="n">
-        <v>3022.8</v>
+        <v>100</v>
       </c>
       <c r="M3" s="14" t="n">
         <v>816.16</v>
       </c>
       <c r="N3" s="14" t="n">
-        <v>3838.96</v>
+        <f aca="false">+L3*1.27</f>
+        <v>127</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>1</v>
@@ -4162,7 +4165,7 @@
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>21115047</v>
+        <v>21115046</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>22</v>
@@ -4195,13 +4198,14 @@
         <v>27</v>
       </c>
       <c r="L4" s="14" t="n">
-        <v>1204.5</v>
+        <v>200</v>
       </c>
       <c r="M4" s="14" t="n">
         <v>325.22</v>
       </c>
       <c r="N4" s="14" t="n">
-        <v>1529.72</v>
+        <f aca="false">+L4*1.27</f>
+        <v>254</v>
       </c>
       <c r="O4" s="11" t="s">
         <v>1</v>

</xml_diff>